<commit_message>
Medications quick change per Brandie H., LOCUS WIP part 2
</commit_message>
<xml_diff>
--- a/UM/UM_Desc_MDCH_2015.xlsx
+++ b/UM/UM_Desc_MDCH_2015.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25125" windowHeight="15585" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="20580" windowHeight="11640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="desc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">desc!$A$1:$C$101</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="175">
   <si>
     <t>State Svc Desc</t>
   </si>
@@ -524,6 +527,27 @@
   </si>
   <si>
     <t xml:space="preserve">Therapy | Behavioral </t>
+  </si>
+  <si>
+    <t>S0280</t>
+  </si>
+  <si>
+    <t>S0315</t>
+  </si>
+  <si>
+    <t>S0316</t>
+  </si>
+  <si>
+    <t>S9470</t>
+  </si>
+  <si>
+    <t>Disease Mgmt Prog</t>
+  </si>
+  <si>
+    <t>Medical Home Prog</t>
+  </si>
+  <si>
+    <t>Health | Dietician Svcs</t>
   </si>
 </sst>
 </file>
@@ -905,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1879,6 +1903,38 @@
         <v>167</v>
       </c>
     </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>168</v>
+      </c>
+      <c r="C102" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>169</v>
+      </c>
+      <c r="C103" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>170</v>
+      </c>
+      <c r="C104" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>171</v>
+      </c>
+      <c r="C105" t="s">
+        <v>174</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>